<commit_message>
adjusting the Exp_Setting column
</commit_message>
<xml_diff>
--- a/inst/extdata/Curated_datasets.xlsx
+++ b/inst/extdata/Curated_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmedsalah/DoReMiTra/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA41BF3A-7812-0946-ADAA-9F77A193E284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F9CD8F-851D-2945-AC7C-0A9581D753D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{70D3F6C7-018C-1D43-8B93-4E2D6206F13E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="221">
   <si>
     <t>Repository</t>
   </si>
@@ -141,12 +141,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>0, 2, 5, 6 and 7</t>
-  </si>
-  <si>
-    <t>24h</t>
-  </si>
-  <si>
     <t>GSE97000</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>lymphocytes</t>
   </si>
   <si>
-    <t>0 and 2</t>
-  </si>
-  <si>
     <t>GSE44201</t>
   </si>
   <si>
@@ -171,15 +162,9 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE44201</t>
   </si>
   <si>
-    <t>vitro</t>
-  </si>
-  <si>
     <t>0. 0.5, 2, 5, or 8 Gy</t>
   </si>
   <si>
-    <t>6, 24, 48h</t>
-  </si>
-  <si>
     <t>GSE43151</t>
   </si>
   <si>
@@ -189,9 +174,6 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE43151</t>
   </si>
   <si>
-    <t>500,100,50,25,10 and 5 mGy</t>
-  </si>
-  <si>
     <t>150, 300, 450 and 600 min</t>
   </si>
   <si>
@@ -210,9 +192,6 @@
     <t>PBL</t>
   </si>
   <si>
-    <t>2gy</t>
-  </si>
-  <si>
     <t>Modeled Microgravity</t>
   </si>
   <si>
@@ -228,9 +207,6 @@
     <t>0, 0.1, 0.5, or 2 Gy</t>
   </si>
   <si>
-    <t>6h</t>
-  </si>
-  <si>
     <t>smokers</t>
   </si>
   <si>
@@ -241,12 +217,6 @@
   </si>
   <si>
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE6978</t>
-  </si>
-  <si>
-    <t>0. 0.05, and 0.5 Gy</t>
-  </si>
-  <si>
-    <t>3 and 24h</t>
   </si>
   <si>
     <r>
@@ -272,12 +242,6 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE63952</t>
   </si>
   <si>
-    <t>0 Gy, 0.15 Gy, 0.30 Gy and 1.5 Gy</t>
-  </si>
-  <si>
-    <t>1 h, 2 h , and 6 h</t>
-  </si>
-  <si>
     <t>not all samples were incubated for 6 h</t>
   </si>
   <si>
@@ -290,12 +254,6 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE8917</t>
   </si>
   <si>
-    <t>0.5, 2, 5, 8</t>
-  </si>
-  <si>
-    <t>6 or 24 hours</t>
-  </si>
-  <si>
     <t>GSE36355</t>
   </si>
   <si>
@@ -329,12 +287,6 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE64375</t>
   </si>
   <si>
-    <t>0 Gy, 0.3 Gy, 1.5 Gy and 3.0 Gy</t>
-  </si>
-  <si>
-    <t>1 h</t>
-  </si>
-  <si>
     <t>GSE55953</t>
   </si>
   <si>
@@ -347,9 +299,6 @@
     <t>60 Gy</t>
   </si>
   <si>
-    <t>2, 4 and 20 h</t>
-  </si>
-  <si>
     <t>GSE113509</t>
   </si>
   <si>
@@ -362,9 +311,6 @@
     <t>0.75 Gy</t>
   </si>
   <si>
-    <t>7d</t>
-  </si>
-  <si>
     <t>part of the study has xray exposure, other samples contain mixed feilds</t>
   </si>
   <si>
@@ -378,12 +324,6 @@
   </si>
   <si>
     <t>Neutron</t>
-  </si>
-  <si>
-    <t>0.25 Gy and 1 Gy</t>
-  </si>
-  <si>
-    <t>1,3,7 days</t>
   </si>
   <si>
     <t>part of the study has xray exposure, other samples were exposed to xray</t>
@@ -429,9 +369,6 @@
 </t>
   </si>
   <si>
-    <t>1, 2, and 4</t>
-  </si>
-  <si>
     <t>part of the study has xray exposure, other samples were exposed to neutron</t>
   </si>
   <si>
@@ -444,9 +381,6 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE65292</t>
   </si>
   <si>
-    <t>0.56, 2.23, 4.45</t>
-  </si>
-  <si>
     <t>GSE15341</t>
   </si>
   <si>
@@ -471,9 +405,6 @@
     <t>various diseases</t>
   </si>
   <si>
-    <t>1.25, 3.75</t>
-  </si>
-  <si>
     <t>GSE196400</t>
   </si>
   <si>
@@ -567,9 +498,6 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE101402</t>
   </si>
   <si>
-    <t>6, 8.8Gy</t>
-  </si>
-  <si>
     <t>Parp1-/- or wild-type mice were either exposed to a LD50/30 dose of x rays</t>
   </si>
   <si>
@@ -582,15 +510,9 @@
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE99176</t>
   </si>
   <si>
-    <t>3,4,8 Gy</t>
-  </si>
-  <si>
     <t>Three genotypes (wild-type, ATM-/-, and Scid) were exposed to a LD50/30 dose</t>
   </si>
   <si>
-    <t>1 Gy and 4 Gy</t>
-  </si>
-  <si>
     <t>1,3,7 d</t>
   </si>
   <si>
@@ -621,12 +543,6 @@
     <t>Macaca mulatta</t>
   </si>
   <si>
-    <t>vivo</t>
-  </si>
-  <si>
-    <t>10.1Gy total</t>
-  </si>
-  <si>
     <t>2, 5 and 30 d</t>
   </si>
   <si>
@@ -645,12 +561,6 @@
     <t>Homo sapiens</t>
   </si>
   <si>
-    <t>4h, 24h</t>
-  </si>
-  <si>
-    <t>4h</t>
-  </si>
-  <si>
     <t>Whole blood</t>
   </si>
   <si>
@@ -709,13 +619,109 @@
   </si>
   <si>
     <t>Girardi</t>
+  </si>
+  <si>
+    <t>0, 2, 5, 6 or 7 Gy</t>
+  </si>
+  <si>
+    <t>0 or 2 Gy</t>
+  </si>
+  <si>
+    <t>500,100,50,25,10 or 5 mGy</t>
+  </si>
+  <si>
+    <t>2 Gy</t>
+  </si>
+  <si>
+    <t>0. 0.05, or 0.5 Gy</t>
+  </si>
+  <si>
+    <t>0 Gy, 0.15 Gy, 0.30 Gy or 1.5 Gy</t>
+  </si>
+  <si>
+    <t>0.5, 2, 5, 8 Gy</t>
+  </si>
+  <si>
+    <t>1 Gy</t>
+  </si>
+  <si>
+    <t>0 Gy, 0.3 Gy, 1.5 Gy or 3 Gy</t>
+  </si>
+  <si>
+    <t>0.25 Gy or 1 Gy</t>
+  </si>
+  <si>
+    <t>1, 2, or 4 Gy</t>
+  </si>
+  <si>
+    <t>0.56, 2.23, 4.45 Gy</t>
+  </si>
+  <si>
+    <t>1.25, 3.75 Gy</t>
+  </si>
+  <si>
+    <t>1 Gy or 4 Gy</t>
+  </si>
+  <si>
+    <t>3, 4, or 8 Gy</t>
+  </si>
+  <si>
+    <t>6, or 8.8 Gy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1Gy </t>
+  </si>
+  <si>
+    <t>24hr</t>
+  </si>
+  <si>
+    <t>6, 24, 48hr</t>
+  </si>
+  <si>
+    <t>24 hr</t>
+  </si>
+  <si>
+    <t>6 hr</t>
+  </si>
+  <si>
+    <t>3 and 24 hr</t>
+  </si>
+  <si>
+    <t>1 h, 2, and 6 hr</t>
+  </si>
+  <si>
+    <t>6 or 24 hr</t>
+  </si>
+  <si>
+    <t>0.5 hr</t>
+  </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>2, 4 and 20 hr</t>
+  </si>
+  <si>
+    <t>7 d</t>
+  </si>
+  <si>
+    <t>4 hr</t>
+  </si>
+  <si>
+    <t>4, 24 hr</t>
+  </si>
+  <si>
+    <t>InVivo</t>
+  </si>
+  <si>
+    <t>ExVivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -748,6 +754,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -783,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -801,6 +813,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1140,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A32738-E9BB-EF47-95D2-AC29DAD18F60}">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1171,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1180,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1201,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>9</v>
@@ -1233,13 +1248,13 @@
         <v>2019</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H2" s="2">
         <v>248</v>
@@ -1251,10 +1266,10 @@
         <v>19</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>32</v>
@@ -1284,13 +1299,13 @@
         <v>2018</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H3" s="2">
         <v>48</v>
@@ -1302,10 +1317,10 @@
         <v>19</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>32</v>
@@ -1337,13 +1352,13 @@
         <v>2017</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="H4" s="2">
         <v>167</v>
@@ -1355,10 +1370,10 @@
         <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>32</v>
@@ -1367,10 +1382,10 @@
         <v>20</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>33</v>
+        <v>189</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
@@ -1379,22 +1394,22 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2">
         <v>2017</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H5" s="2">
         <v>12</v>
@@ -1406,10 +1421,10 @@
         <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>32</v>
@@ -1418,10 +1433,10 @@
         <v>20</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>39</v>
+        <v>190</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q5" s="2"/>
     </row>
@@ -1430,22 +1445,22 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2">
         <v>2013</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H6" s="2">
         <v>75</v>
@@ -1457,10 +1472,10 @@
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>32</v>
@@ -1469,10 +1484,10 @@
         <v>20</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="Q6" s="2"/>
     </row>
@@ -1481,22 +1496,22 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2">
         <v>2013</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H7" s="2">
         <v>121</v>
@@ -1508,10 +1523,10 @@
         <v>19</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>32</v>
@@ -1520,13 +1535,13 @@
         <v>20</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>49</v>
+        <v>191</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1534,22 +1549,22 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2">
         <v>2012</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H8" s="2">
         <v>20</v>
@@ -1561,10 +1576,10 @@
         <v>19</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>32</v>
@@ -1573,13 +1588,13 @@
         <v>20</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>56</v>
+        <v>192</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1587,22 +1602,22 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2">
         <v>2011</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H9" s="2">
         <v>95</v>
@@ -1614,10 +1629,10 @@
         <v>19</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>32</v>
@@ -1626,13 +1641,13 @@
         <v>20</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>62</v>
+        <v>209</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1640,22 +1655,22 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2">
         <v>2008</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H10" s="2">
         <v>114</v>
@@ -1667,10 +1682,10 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>32</v>
@@ -1679,13 +1694,13 @@
         <v>20</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>68</v>
+        <v>210</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -1693,22 +1708,22 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2">
         <v>2019</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H11" s="2">
         <v>100</v>
@@ -1720,10 +1735,10 @@
         <v>19</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>32</v>
@@ -1732,13 +1747,13 @@
         <v>20</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>73</v>
+        <v>194</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -1746,22 +1761,22 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D12" s="2">
         <v>2008</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H12" s="2">
         <v>50</v>
@@ -1773,10 +1788,10 @@
         <v>19</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>32</v>
@@ -1785,10 +1800,10 @@
         <v>20</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>79</v>
+        <v>195</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>80</v>
+        <v>212</v>
       </c>
       <c r="Q12" s="2"/>
     </row>
@@ -1797,22 +1812,22 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2">
         <v>2014</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H13" s="2">
         <v>16</v>
@@ -1824,10 +1839,10 @@
         <v>19</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>32</v>
@@ -1835,11 +1850,11 @@
       <c r="N13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="2">
-        <v>1</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0.5</v>
+      <c r="O13" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="Q13" s="2"/>
     </row>
@@ -1848,22 +1863,22 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D14" s="2">
         <v>2013</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H14" s="2">
         <v>6</v>
@@ -1875,10 +1890,10 @@
         <v>19</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>32</v>
@@ -1887,10 +1902,10 @@
         <v>20</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q14" s="2"/>
     </row>
@@ -1899,22 +1914,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2">
         <v>2015</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H15" s="2">
         <v>16</v>
@@ -1926,10 +1941,10 @@
         <v>19</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>32</v>
@@ -1938,10 +1953,10 @@
         <v>20</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="Q15" s="2"/>
     </row>
@@ -1950,22 +1965,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2">
         <v>2015</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H16" s="2">
         <v>28</v>
@@ -1977,10 +1992,10 @@
         <v>19</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>32</v>
@@ -1989,10 +2004,10 @@
         <v>20</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>98</v>
+        <v>215</v>
       </c>
       <c r="Q16" s="2"/>
     </row>
@@ -2001,22 +2016,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D17" s="2">
         <v>2018</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H17" s="2">
         <v>12</v>
@@ -2028,25 +2043,25 @@
         <v>19</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -2054,22 +2069,22 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D18" s="2">
         <v>2017</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H18" s="2">
         <v>45</v>
@@ -2081,25 +2096,25 @@
         <v>19</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -2107,22 +2122,22 @@
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D19" s="2">
         <v>2017</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H19" s="2">
         <v>51</v>
@@ -2134,22 +2149,22 @@
         <v>19</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q19" s="2"/>
     </row>
@@ -2158,22 +2173,22 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="D20" s="2">
         <v>2010</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H20" s="2">
         <v>16</v>
@@ -2182,28 +2197,28 @@
         <v>18</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -2211,22 +2226,22 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D21" s="2">
         <v>2017</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H21" s="2">
         <v>52</v>
@@ -2238,25 +2253,25 @@
         <v>19</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -2264,22 +2279,22 @@
         <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="D22" s="2">
         <v>2015</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H22" s="2">
         <v>35</v>
@@ -2291,22 +2306,22 @@
         <v>19</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q22" s="2"/>
     </row>
@@ -2315,22 +2330,22 @@
         <v>14</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="D23" s="2">
         <v>2009</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H23" s="2">
         <v>24</v>
@@ -2342,25 +2357,25 @@
         <v>19</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="O23" s="2">
-        <v>2</v>
+        <v>101</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -2368,22 +2383,22 @@
         <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="D24" s="2">
         <v>2011</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H24" s="2">
         <v>66</v>
@@ -2392,25 +2407,25 @@
         <v>18</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>139</v>
+        <v>201</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="Q24" s="2"/>
     </row>
@@ -2419,22 +2434,22 @@
         <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="D25" s="2">
         <v>2023</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H25" s="2">
         <v>24</v>
@@ -2446,25 +2461,25 @@
         <v>19</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q25" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -2472,22 +2487,22 @@
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="D26" s="2">
         <v>2022</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H26" s="2">
         <v>30</v>
@@ -2499,25 +2514,25 @@
         <v>19</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -2525,22 +2540,22 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="D27" s="2">
         <v>2021</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H27" s="2">
         <v>24</v>
@@ -2552,25 +2567,25 @@
         <v>19</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -2578,22 +2593,22 @@
         <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="D28" s="2">
         <v>2020</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H28" s="2">
         <v>17</v>
@@ -2605,25 +2620,25 @@
         <v>19</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -2631,22 +2646,22 @@
         <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="D29" s="2">
         <v>2019</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H29" s="2">
         <v>20</v>
@@ -2658,25 +2673,25 @@
         <v>19</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -2684,22 +2699,22 @@
         <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D30" s="2">
         <v>2018</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H30" s="2">
         <v>12</v>
@@ -2711,25 +2726,25 @@
         <v>19</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -2737,22 +2752,22 @@
         <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="D31" s="2">
         <v>2018</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H31" s="2">
         <v>24</v>
@@ -2764,25 +2779,25 @@
         <v>19</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
@@ -2790,22 +2805,22 @@
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="D32" s="2">
         <v>2018</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H32" s="2">
         <v>32</v>
@@ -2817,25 +2832,25 @@
         <v>19</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -2843,22 +2858,22 @@
         <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D33" s="2">
         <v>2017</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H33" s="2">
         <v>43</v>
@@ -2870,25 +2885,25 @@
         <v>19</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -2896,22 +2911,22 @@
         <v>14</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="D34" s="2">
         <v>2015</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H34" s="2">
         <v>48</v>
@@ -2923,25 +2938,25 @@
         <v>19</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>34</v>
+        <v>157</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -2949,22 +2964,22 @@
         <v>14</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="D35" s="2">
         <v>2018</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="H35" s="2">
         <v>20</v>
@@ -2976,25 +2991,25 @@
         <v>19</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -3002,22 +3017,22 @@
         <v>14</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="D36" s="2">
         <v>2021</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H36" s="2">
         <v>20</v>
@@ -3029,22 +3044,22 @@
         <v>19</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>34</v>
+        <v>129</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="Q36" s="2"/>
     </row>

</xml_diff>

<commit_message>
adjust some names from capital to small letters
</commit_message>
<xml_diff>
--- a/inst/extdata/Curated_datasets.xlsx
+++ b/inst/extdata/Curated_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmedsalah/DoReMiTra/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F9CD8F-851D-2945-AC7C-0A9581D753D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFEF983-8AD6-D34D-B30C-19EFE0F065F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{70D3F6C7-018C-1D43-8B93-4E2D6206F13E}"/>
   </bookViews>
@@ -579,18 +579,9 @@
     <t>Paul</t>
   </si>
   <si>
-    <t>NOSEL</t>
-  </si>
-  <si>
-    <t>GRUEL</t>
-  </si>
-  <si>
     <t>Rouchka</t>
   </si>
   <si>
-    <t>MANIKANDAN</t>
-  </si>
-  <si>
     <t>Lee</t>
   </si>
   <si>
@@ -715,6 +706,15 @@
   </si>
   <si>
     <t>ExVivo</t>
+  </si>
+  <si>
+    <t>Gruel</t>
+  </si>
+  <si>
+    <t>Manikandan</t>
+  </si>
+  <si>
+    <t>Nosel</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1156,7 @@
   <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>9</v>
@@ -1269,7 +1269,7 @@
         <v>169</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>32</v>
@@ -1320,7 +1320,7 @@
         <v>169</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>32</v>
@@ -1373,7 +1373,7 @@
         <v>169</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>32</v>
@@ -1382,10 +1382,10 @@
         <v>20</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
@@ -1403,7 +1403,7 @@
         <v>2017</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>35</v>
@@ -1424,7 +1424,7 @@
         <v>36</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>32</v>
@@ -1433,10 +1433,10 @@
         <v>20</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q5" s="2"/>
     </row>
@@ -1475,7 +1475,7 @@
         <v>169</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>32</v>
@@ -1487,7 +1487,7 @@
         <v>40</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="Q6" s="2"/>
     </row>
@@ -1505,7 +1505,7 @@
         <v>2013</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>43</v>
@@ -1526,7 +1526,7 @@
         <v>169</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>32</v>
@@ -1535,7 +1535,7 @@
         <v>20</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>44</v>
@@ -1558,7 +1558,7 @@
         <v>2012</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>48</v>
@@ -1579,7 +1579,7 @@
         <v>49</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>32</v>
@@ -1588,10 +1588,10 @@
         <v>20</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>50</v>
@@ -1632,7 +1632,7 @@
         <v>169</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>32</v>
@@ -1644,7 +1644,7 @@
         <v>54</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>55</v>
@@ -1664,7 +1664,7 @@
         <v>2008</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>58</v>
@@ -1685,7 +1685,7 @@
         <v>169</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>32</v>
@@ -1694,10 +1694,10 @@
         <v>20</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>59</v>
@@ -1717,7 +1717,7 @@
         <v>2019</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>62</v>
@@ -1738,7 +1738,7 @@
         <v>169</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>32</v>
@@ -1747,10 +1747,10 @@
         <v>20</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>63</v>
@@ -1791,7 +1791,7 @@
         <v>169</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>32</v>
@@ -1800,10 +1800,10 @@
         <v>20</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q12" s="2"/>
     </row>
@@ -1821,7 +1821,7 @@
         <v>2014</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>69</v>
@@ -1842,7 +1842,7 @@
         <v>70</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>32</v>
@@ -1851,10 +1851,10 @@
         <v>20</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="Q13" s="2"/>
     </row>
@@ -1872,7 +1872,7 @@
         <v>2013</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>73</v>
@@ -1893,7 +1893,7 @@
         <v>70</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>32</v>
@@ -1905,7 +1905,7 @@
         <v>74</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q14" s="2"/>
     </row>
@@ -1923,7 +1923,7 @@
         <v>2015</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>77</v>
@@ -1944,7 +1944,7 @@
         <v>169</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>32</v>
@@ -1953,10 +1953,10 @@
         <v>20</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="Q15" s="2"/>
     </row>
@@ -1974,7 +1974,7 @@
         <v>2015</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>80</v>
@@ -1995,7 +1995,7 @@
         <v>70</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>32</v>
@@ -2007,7 +2007,7 @@
         <v>81</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q16" s="2"/>
     </row>
@@ -2025,7 +2025,7 @@
         <v>2018</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>84</v>
@@ -2046,7 +2046,7 @@
         <v>169</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>32</v>
@@ -2058,7 +2058,7 @@
         <v>85</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>86</v>
@@ -2078,7 +2078,7 @@
         <v>2017</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>89</v>
@@ -2099,7 +2099,7 @@
         <v>169</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>32</v>
@@ -2108,7 +2108,7 @@
         <v>90</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>153</v>
@@ -2131,7 +2131,7 @@
         <v>2017</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>94</v>
@@ -2152,7 +2152,7 @@
         <v>169</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>32</v>
@@ -2164,7 +2164,7 @@
         <v>95</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q19" s="2"/>
     </row>
@@ -2203,7 +2203,7 @@
         <v>169</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>100</v>
@@ -2215,7 +2215,7 @@
         <v>102</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>103</v>
@@ -2235,7 +2235,7 @@
         <v>2017</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>94</v>
@@ -2256,7 +2256,7 @@
         <v>169</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>32</v>
@@ -2265,10 +2265,10 @@
         <v>101</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Q21" s="2" t="s">
         <v>105</v>
@@ -2288,7 +2288,7 @@
         <v>2015</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>108</v>
@@ -2309,7 +2309,7 @@
         <v>169</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>32</v>
@@ -2318,10 +2318,10 @@
         <v>101</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q22" s="2"/>
     </row>
@@ -2339,7 +2339,7 @@
         <v>2009</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>111</v>
@@ -2360,7 +2360,7 @@
         <v>70</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>32</v>
@@ -2369,10 +2369,10 @@
         <v>101</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>112</v>
@@ -2413,7 +2413,7 @@
         <v>169</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>116</v>
@@ -2422,10 +2422,10 @@
         <v>101</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="Q24" s="2"/>
     </row>
@@ -2443,7 +2443,7 @@
         <v>2023</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>119</v>
@@ -2464,7 +2464,7 @@
         <v>169</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>32</v>
@@ -2476,7 +2476,7 @@
         <v>120</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>121</v>
@@ -2496,7 +2496,7 @@
         <v>2022</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>124</v>
@@ -2517,7 +2517,7 @@
         <v>169</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>32</v>
@@ -2529,7 +2529,7 @@
         <v>120</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>125</v>
@@ -2549,7 +2549,7 @@
         <v>2021</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>132</v>
@@ -2570,7 +2570,7 @@
         <v>169</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>32</v>
@@ -2582,7 +2582,7 @@
         <v>129</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>133</v>
@@ -2602,7 +2602,7 @@
         <v>2020</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>136</v>
@@ -2623,7 +2623,7 @@
         <v>169</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>32</v>
@@ -2635,7 +2635,7 @@
         <v>137</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>138</v>
@@ -2655,7 +2655,7 @@
         <v>2019</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>141</v>
@@ -2676,7 +2676,7 @@
         <v>169</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>32</v>
@@ -2688,7 +2688,7 @@
         <v>142</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>143</v>
@@ -2708,7 +2708,7 @@
         <v>2018</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>84</v>
@@ -2729,7 +2729,7 @@
         <v>169</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>32</v>
@@ -2741,7 +2741,7 @@
         <v>144</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>86</v>
@@ -2782,7 +2782,7 @@
         <v>169</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>32</v>
@@ -2791,10 +2791,10 @@
         <v>101</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>148</v>
@@ -2835,7 +2835,7 @@
         <v>169</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>32</v>
@@ -2844,10 +2844,10 @@
         <v>101</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>152</v>
@@ -2867,7 +2867,7 @@
         <v>2017</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>89</v>
@@ -2888,7 +2888,7 @@
         <v>169</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>32</v>
@@ -2897,7 +2897,7 @@
         <v>101</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="P33" s="2" t="s">
         <v>153</v>
@@ -2941,7 +2941,7 @@
         <v>169</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>32</v>
@@ -2953,7 +2953,7 @@
         <v>157</v>
       </c>
       <c r="P34" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>158</v>
@@ -2973,7 +2973,7 @@
         <v>2018</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>161</v>
@@ -2994,7 +2994,7 @@
         <v>169</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>32</v>
@@ -3003,7 +3003,7 @@
         <v>101</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="P35" s="2" t="s">
         <v>163</v>
@@ -3026,7 +3026,7 @@
         <v>2021</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>128</v>
@@ -3047,7 +3047,7 @@
         <v>169</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>32</v>
@@ -3059,7 +3059,7 @@
         <v>129</v>
       </c>
       <c r="P36" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Q36" s="2"/>
     </row>
@@ -3295,18 +3295,18 @@
     <hyperlink ref="F4" r:id="rId3" xr:uid="{AFF75824-9BB1-3E43-821E-53421CF5E1AF}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{38A2E2D3-5921-3740-99B7-B4277C1EC967}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{4E4FD863-EC59-B645-8821-21770B6B0961}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{40A8091E-33D1-9D41-97B7-4638960E3F4A}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{6A4401F3-AC2B-1842-96E3-E8442ADD1A75}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{0B5CA78E-2C54-A74A-87E0-C68F7F0E63FE}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{C9F53D9C-3785-C040-9209-8012669E5766}"/>
-    <hyperlink ref="F14" r:id="rId10" xr:uid="{341FA7E5-90B8-AD4C-A0BE-2A9A93EF1520}"/>
-    <hyperlink ref="F18" r:id="rId11" xr:uid="{36FFFBC1-EE7A-E741-8EB5-8CF628638045}"/>
-    <hyperlink ref="F19" r:id="rId12" xr:uid="{A792E33F-294D-2445-AB05-CB907A07959E}"/>
-    <hyperlink ref="F35" r:id="rId13" xr:uid="{8F732B53-D892-2441-8ED5-007250C1B000}"/>
-    <hyperlink ref="F15" r:id="rId14" xr:uid="{8387AEEB-9623-0644-B678-30456CA35BB1}"/>
-    <hyperlink ref="F36" r:id="rId15" xr:uid="{4C251268-4937-1149-8766-98D5012AB07A}"/>
-    <hyperlink ref="F13" r:id="rId16" xr:uid="{FF1CCBFE-0370-724A-B76C-5078EC2A33CC}"/>
-    <hyperlink ref="F27" r:id="rId17" xr:uid="{57A8BEA1-4259-B842-8C28-C7C79B948669}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{6A4401F3-AC2B-1842-96E3-E8442ADD1A75}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{0B5CA78E-2C54-A74A-87E0-C68F7F0E63FE}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{C9F53D9C-3785-C040-9209-8012669E5766}"/>
+    <hyperlink ref="F14" r:id="rId9" xr:uid="{341FA7E5-90B8-AD4C-A0BE-2A9A93EF1520}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{36FFFBC1-EE7A-E741-8EB5-8CF628638045}"/>
+    <hyperlink ref="F19" r:id="rId11" xr:uid="{A792E33F-294D-2445-AB05-CB907A07959E}"/>
+    <hyperlink ref="F35" r:id="rId12" xr:uid="{8F732B53-D892-2441-8ED5-007250C1B000}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{8387AEEB-9623-0644-B678-30456CA35BB1}"/>
+    <hyperlink ref="F36" r:id="rId14" xr:uid="{4C251268-4937-1149-8766-98D5012AB07A}"/>
+    <hyperlink ref="F13" r:id="rId15" xr:uid="{FF1CCBFE-0370-724A-B76C-5078EC2A33CC}"/>
+    <hyperlink ref="F27" r:id="rId16" xr:uid="{57A8BEA1-4259-B842-8C28-C7C79B948669}"/>
+    <hyperlink ref="F7" r:id="rId17" xr:uid="{40A8091E-33D1-9D41-97B7-4638960E3F4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
few fixes on the excel file to have the links fully rendered and removing the color coding
</commit_message>
<xml_diff>
--- a/inst/extdata/Curated_datasets.xlsx
+++ b/inst/extdata/Curated_datasets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmedsalah/DoReMiTra/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fede/Development/DoReMiTra/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFEF983-8AD6-D34D-B30C-19EFE0F065F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42376DF-CF13-734E-B3D3-CF718DAFEC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{70D3F6C7-018C-1D43-8B93-4E2D6206F13E}"/>
   </bookViews>
@@ -762,7 +762,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -772,12 +772,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.749992370372631"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,7 +789,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -809,13 +803,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1155,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A32738-E9BB-EF47-95D2-AC29DAD18F60}">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,7 +1169,7 @@
     <col min="3" max="3" width="108.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -1197,7 +1200,7 @@
       <c r="E1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1250,7 +1253,7 @@
       <c r="E2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1301,7 +1304,7 @@
       <c r="E3" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1354,7 +1357,7 @@
       <c r="E4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1405,7 +1408,7 @@
       <c r="E5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1456,7 +1459,7 @@
       <c r="E6" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1507,7 +1510,7 @@
       <c r="E7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1560,7 +1563,7 @@
       <c r="E8" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="7" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1613,7 +1616,7 @@
       <c r="E9" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1666,7 +1669,7 @@
       <c r="E10" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7" t="s">
         <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1719,7 +1722,7 @@
       <c r="E11" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1772,7 +1775,7 @@
       <c r="E12" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="7" t="s">
         <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1823,7 +1826,7 @@
       <c r="E13" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>69</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -1874,7 +1877,7 @@
       <c r="E14" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="7" t="s">
         <v>73</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1913,7 +1916,7 @@
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="10" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1925,7 +1928,7 @@
       <c r="E15" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="7" t="s">
         <v>77</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -1976,7 +1979,7 @@
       <c r="E16" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="7" t="s">
         <v>80</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -2027,7 +2030,7 @@
       <c r="E17" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -2080,7 +2083,7 @@
       <c r="E18" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -2133,7 +2136,7 @@
       <c r="E19" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="7" t="s">
         <v>94</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -2184,7 +2187,7 @@
       <c r="E20" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="7" t="s">
         <v>98</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -2237,7 +2240,7 @@
       <c r="E21" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="7" t="s">
         <v>94</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -2290,7 +2293,7 @@
       <c r="E22" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="7" t="s">
         <v>108</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -2329,7 +2332,7 @@
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="10" t="s">
         <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -2341,7 +2344,7 @@
       <c r="E23" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="7" t="s">
         <v>111</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -2394,7 +2397,7 @@
       <c r="E24" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="7" t="s">
         <v>115</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2445,7 +2448,7 @@
       <c r="E25" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="7" t="s">
         <v>119</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -2498,7 +2501,7 @@
       <c r="E26" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="7" t="s">
         <v>124</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -2551,7 +2554,7 @@
       <c r="E27" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="7" t="s">
         <v>132</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -2604,7 +2607,7 @@
       <c r="E28" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="7" t="s">
         <v>136</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -2657,7 +2660,7 @@
       <c r="E29" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="7" t="s">
         <v>141</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -2710,7 +2713,7 @@
       <c r="E30" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -2763,7 +2766,7 @@
       <c r="E31" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="7" t="s">
         <v>147</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -2816,7 +2819,7 @@
       <c r="E32" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="7" t="s">
         <v>151</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -2869,7 +2872,7 @@
       <c r="E33" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -2922,7 +2925,7 @@
       <c r="E34" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="7" t="s">
         <v>156</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -2952,7 +2955,7 @@
       <c r="O34" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="P34" s="7" t="s">
+      <c r="P34" s="5" t="s">
         <v>205</v>
       </c>
       <c r="Q34" s="2" t="s">
@@ -2975,7 +2978,7 @@
       <c r="E35" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="7" t="s">
         <v>161</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -3028,7 +3031,7 @@
       <c r="E36" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="7" t="s">
         <v>128</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -3058,7 +3061,7 @@
       <c r="O36" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="P36" s="7" t="s">
+      <c r="P36" s="5" t="s">
         <v>205</v>
       </c>
       <c r="Q36" s="2"/>
@@ -3067,7 +3070,7 @@
       <c r="B37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="F37" s="8"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -3082,7 +3085,7 @@
       <c r="B38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="F38" s="8"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -3097,7 +3100,7 @@
       <c r="B39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="8"/>
       <c r="H39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -3108,7 +3111,7 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="F40" s="8"/>
       <c r="H40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -3118,7 +3121,7 @@
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="F41" s="8"/>
       <c r="H41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -3128,7 +3131,7 @@
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="F42" s="8"/>
       <c r="H42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -3137,7 +3140,7 @@
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="F43" s="8"/>
       <c r="H43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
@@ -3146,7 +3149,7 @@
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="F44" s="8"/>
       <c r="H44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -3155,137 +3158,137 @@
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="F45" s="8"/>
       <c r="L45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="F48" s="8"/>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="F49" s="8"/>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
+      <c r="F50" s="8"/>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
+      <c r="F51" s="8"/>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="F52" s="8"/>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+      <c r="F53" s="8"/>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="F54" s="8"/>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="F55" s="8"/>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+      <c r="F56" s="8"/>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
+      <c r="F57" s="8"/>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="F58" s="8"/>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="F59" s="8"/>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="F60" s="8"/>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="F61" s="8"/>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F62" s="2"/>
+      <c r="F62" s="8"/>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F63" s="2"/>
+      <c r="F63" s="8"/>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F64" s="2"/>
+      <c r="F64" s="8"/>
     </row>
     <row r="65" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F65" s="2"/>
+      <c r="F65" s="8"/>
     </row>
     <row r="66" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F66" s="2"/>
+      <c r="F66" s="8"/>
     </row>
     <row r="67" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F67" s="2"/>
+      <c r="F67" s="8"/>
     </row>
     <row r="68" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F68" s="2"/>
+      <c r="F68" s="8"/>
     </row>
     <row r="69" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F69" s="2"/>
+      <c r="F69" s="8"/>
     </row>
     <row r="70" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F70" s="2"/>
+      <c r="F70" s="8"/>
     </row>
     <row r="71" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F71" s="2"/>
+      <c r="F71" s="8"/>
     </row>
     <row r="72" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F72" s="2"/>
+      <c r="F72" s="8"/>
     </row>
     <row r="73" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F73" s="2"/>
+      <c r="F73" s="8"/>
     </row>
     <row r="74" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F74" s="2"/>
+      <c r="F74" s="8"/>
     </row>
     <row r="75" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F75" s="2"/>
+      <c r="F75" s="8"/>
     </row>
     <row r="76" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F76" s="2"/>
+      <c r="F76" s="8"/>
     </row>
     <row r="77" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F77" s="2"/>
+      <c r="F77" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="L1:L77" xr:uid="{67A32738-E9BB-EF47-95D2-AC29DAD18F60}"/>
@@ -3307,6 +3310,24 @@
     <hyperlink ref="F13" r:id="rId15" xr:uid="{FF1CCBFE-0370-724A-B76C-5078EC2A33CC}"/>
     <hyperlink ref="F27" r:id="rId16" xr:uid="{57A8BEA1-4259-B842-8C28-C7C79B948669}"/>
     <hyperlink ref="F7" r:id="rId17" xr:uid="{40A8091E-33D1-9D41-97B7-4638960E3F4A}"/>
+    <hyperlink ref="F11" r:id="rId18" xr:uid="{51948A1B-DC0E-384F-8B34-79DD17E1D8F9}"/>
+    <hyperlink ref="F12" r:id="rId19" xr:uid="{542AD18D-19EC-164C-8CF5-B495FAD607C2}"/>
+    <hyperlink ref="F16" r:id="rId20" xr:uid="{27678B7B-B947-3A48-8BEE-974F65A4C02F}"/>
+    <hyperlink ref="F17" r:id="rId21" xr:uid="{3D013BB4-CF33-6148-8CCB-B240269BC1BE}"/>
+    <hyperlink ref="F20" r:id="rId22" xr:uid="{6E58A1CF-1F6F-904C-9EAE-823F157EFB18}"/>
+    <hyperlink ref="F21" r:id="rId23" xr:uid="{A9360C8E-AE98-B54B-89AB-EB2856F4AF8E}"/>
+    <hyperlink ref="F22" r:id="rId24" xr:uid="{325D3A52-06EA-EB4A-B52D-213699641008}"/>
+    <hyperlink ref="F23" r:id="rId25" xr:uid="{E00C0782-A607-2846-B53B-72A3169A92DE}"/>
+    <hyperlink ref="F24" r:id="rId26" xr:uid="{8E8FD726-8E5C-DA4E-A924-FFA71234138C}"/>
+    <hyperlink ref="F25" r:id="rId27" xr:uid="{E08D3645-ED59-BC41-8CF2-206FE98BB3FE}"/>
+    <hyperlink ref="F26" r:id="rId28" xr:uid="{7258473D-2E30-B84F-AC67-BDAEBC015CDB}"/>
+    <hyperlink ref="F28" r:id="rId29" xr:uid="{F3B0F188-D828-6B44-AC1E-B1D2186EDC11}"/>
+    <hyperlink ref="F29" r:id="rId30" xr:uid="{E18936CE-F435-B144-B840-32DACD2FD86A}"/>
+    <hyperlink ref="F30" r:id="rId31" xr:uid="{6C61F990-23B8-C14D-8987-FFC837944BF1}"/>
+    <hyperlink ref="F31" r:id="rId32" xr:uid="{0106454A-0EC1-C949-AF97-FB33C07FC161}"/>
+    <hyperlink ref="F32" r:id="rId33" xr:uid="{D84F3501-217A-BF4F-AE0A-793C35A189FB}"/>
+    <hyperlink ref="F33" r:id="rId34" xr:uid="{DE626974-B42C-D844-8516-D08AC4DAE166}"/>
+    <hyperlink ref="F34" r:id="rId35" xr:uid="{0E32C1BB-3618-FC46-9550-9045A736B598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>